<commit_message>
Fate fell short this time
</commit_message>
<xml_diff>
--- a/Time-table.xlsx
+++ b/Time-table.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6E25FA-6635-472D-A596-60C1F75E2C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rooms" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="228">
   <si>
     <t>Class</t>
   </si>
@@ -699,13 +700,16 @@
   </si>
   <si>
     <t>Kartik Konar, Sulaxan</t>
+  </si>
+  <si>
+    <t>Shilpa Marathe B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -739,6 +743,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -766,7 +776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -803,6 +813,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -896,6 +907,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -931,6 +959,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1106,17 +1151,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>216</v>
       </c>
@@ -1127,7 +1172,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>306</v>
       </c>
@@ -1138,7 +1183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>313</v>
       </c>
@@ -1149,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>341</v>
       </c>
@@ -1160,7 +1205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>328</v>
       </c>
@@ -1171,7 +1216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>329</v>
       </c>
@@ -1182,7 +1227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>330</v>
       </c>
@@ -1193,7 +1238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>331</v>
       </c>
@@ -1204,7 +1249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>332</v>
       </c>
@@ -1215,7 +1260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>333</v>
       </c>
@@ -1226,7 +1271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>334</v>
       </c>
@@ -1237,7 +1282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>336</v>
       </c>
@@ -1248,7 +1293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>338</v>
       </c>
@@ -1259,7 +1304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>339</v>
       </c>
@@ -1270,7 +1315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>337</v>
       </c>
@@ -1281,7 +1326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>305</v>
       </c>
@@ -1292,7 +1337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>314</v>
       </c>
@@ -1303,7 +1348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>335</v>
       </c>
@@ -1314,7 +1359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>406</v>
       </c>
@@ -1325,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>409</v>
       </c>
@@ -1336,7 +1381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>430</v>
       </c>
@@ -1347,7 +1392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>432</v>
       </c>
@@ -1358,7 +1403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>440</v>
       </c>
@@ -1369,7 +1414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>431</v>
       </c>
@@ -1380,7 +1425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>405</v>
       </c>
@@ -1391,7 +1436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>410</v>
       </c>
@@ -1402,7 +1447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>433</v>
       </c>
@@ -1413,7 +1458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>434</v>
       </c>
@@ -1424,7 +1469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>435</v>
       </c>
@@ -1435,7 +1480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>436</v>
       </c>
@@ -1446,7 +1491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>437</v>
       </c>
@@ -1457,7 +1502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>438</v>
       </c>
@@ -1468,7 +1513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>325</v>
       </c>
@@ -1479,7 +1524,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>324</v>
       </c>
@@ -1490,7 +1535,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>353</v>
       </c>
@@ -1501,7 +1546,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>322</v>
       </c>
@@ -1512,7 +1557,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>346</v>
       </c>
@@ -1523,7 +1568,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>326</v>
       </c>
@@ -1534,7 +1579,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>327</v>
       </c>
@@ -1545,7 +1590,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>356</v>
       </c>
@@ -1556,7 +1601,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>354</v>
       </c>
@@ -1567,7 +1612,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>421</v>
       </c>
@@ -1578,7 +1623,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>420</v>
       </c>
@@ -1589,7 +1634,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>413</v>
       </c>
@@ -1600,7 +1645,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>453</v>
       </c>
@@ -1611,7 +1656,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>445</v>
       </c>
@@ -1622,7 +1667,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>446</v>
       </c>
@@ -1633,7 +1678,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>449</v>
       </c>
@@ -1644,7 +1689,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>407</v>
       </c>
@@ -1655,7 +1700,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>408</v>
       </c>
@@ -1666,7 +1711,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>450</v>
       </c>
@@ -1684,27 +1729,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="6" width="22.5546875" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.109375" customWidth="1"/>
-    <col min="14" max="14" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="6" width="22.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>214</v>
       </c>
@@ -1748,7 +1793,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1762,7 +1807,7 @@
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="16" t="s">
         <v>42</v>
       </c>
       <c r="G2" s="1">
@@ -1784,7 +1829,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1798,7 +1843,7 @@
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="16" t="s">
         <v>43</v>
       </c>
       <c r="G3" s="1">
@@ -1820,7 +1865,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1834,7 +1879,7 @@
       <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="16" t="s">
         <v>44</v>
       </c>
       <c r="G4" s="1">
@@ -1856,7 +1901,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1870,7 +1915,7 @@
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="16" t="s">
         <v>45</v>
       </c>
       <c r="G5" s="1">
@@ -1890,7 +1935,7 @@
       </c>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1904,7 +1949,7 @@
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="16" t="s">
         <v>119</v>
       </c>
       <c r="G6" s="1">
@@ -1924,7 +1969,7 @@
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1938,7 +1983,7 @@
       <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="16" t="s">
         <v>47</v>
       </c>
       <c r="G7" s="1">
@@ -1960,7 +2005,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -1974,7 +2019,7 @@
       <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="16" t="s">
         <v>48</v>
       </c>
       <c r="G8" s="1">
@@ -1994,7 +2039,7 @@
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -2008,7 +2053,7 @@
       <c r="E9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="16" t="s">
         <v>49</v>
       </c>
       <c r="G9" s="1">
@@ -2030,7 +2075,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -2044,7 +2089,7 @@
       <c r="E10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="16" t="s">
         <v>50</v>
       </c>
       <c r="G10" s="1">
@@ -2066,7 +2111,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -2080,7 +2125,7 @@
       <c r="E11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="16" t="s">
         <v>43</v>
       </c>
       <c r="G11" s="1">
@@ -2102,7 +2147,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -2116,7 +2161,7 @@
       <c r="E12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="16" t="s">
         <v>119</v>
       </c>
       <c r="G12" s="1">
@@ -2136,7 +2181,7 @@
       </c>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -2150,7 +2195,7 @@
       <c r="E13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="16" t="s">
         <v>119</v>
       </c>
       <c r="G13" s="1">
@@ -2170,7 +2215,7 @@
       </c>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -2186,7 +2231,7 @@
       <c r="E14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="16" t="s">
         <v>112</v>
       </c>
       <c r="G14" s="1">
@@ -2214,7 +2259,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -2230,7 +2275,7 @@
       <c r="E15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="16" t="s">
         <v>107</v>
       </c>
       <c r="G15" s="1">
@@ -2258,7 +2303,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -2274,7 +2319,7 @@
       <c r="E16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="16" t="s">
         <v>108</v>
       </c>
       <c r="G16" s="1">
@@ -2299,7 +2344,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -2315,7 +2360,7 @@
       <c r="E17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="16" t="s">
         <v>109</v>
       </c>
       <c r="G17" s="1">
@@ -2340,7 +2385,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -2356,7 +2401,7 @@
       <c r="E18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="16" t="s">
         <v>110</v>
       </c>
       <c r="G18" s="1">
@@ -2381,7 +2426,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -2397,7 +2442,7 @@
       <c r="E19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="16" t="s">
         <v>111</v>
       </c>
       <c r="G19" s="1">
@@ -2422,7 +2467,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -2438,8 +2483,8 @@
       <c r="E20" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F20" s="11" t="s">
-        <v>111</v>
+      <c r="F20" s="16" t="s">
+        <v>227</v>
       </c>
       <c r="G20" s="1">
         <v>6</v>
@@ -2463,7 +2508,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
@@ -2479,7 +2524,7 @@
       <c r="E21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="16" t="s">
         <v>107</v>
       </c>
       <c r="G21" s="1">
@@ -2504,7 +2549,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
@@ -2520,7 +2565,7 @@
       <c r="E22" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="16" t="s">
         <v>110</v>
       </c>
       <c r="G22" s="1">
@@ -2545,7 +2590,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -2561,7 +2606,7 @@
       <c r="E23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="16" t="s">
         <v>119</v>
       </c>
       <c r="G23" s="1">
@@ -2586,7 +2631,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
@@ -2602,7 +2647,7 @@
       <c r="E24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="16" t="s">
         <v>119</v>
       </c>
       <c r="G24" s="1">
@@ -2625,7 +2670,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
@@ -2671,28 +2716,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
-    <col min="4" max="4" width="41.109375" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" customWidth="1"/>
-    <col min="6" max="6" width="38.5546875" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="41.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="38.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" customWidth="1"/>
-    <col min="14" max="14" width="12.77734375" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>214</v>
       </c>
@@ -2736,7 +2781,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2765,7 +2810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2791,7 +2836,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2817,7 +2862,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2846,7 +2891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2872,7 +2917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -2907,7 +2952,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -2942,7 +2987,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -2971,7 +3016,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -3006,7 +3051,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -3035,7 +3080,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -3067,7 +3112,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -3099,7 +3144,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -3128,7 +3173,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -3160,7 +3205,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>3</v>
       </c>
@@ -3197,7 +3242,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -3232,7 +3277,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -3267,7 +3312,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -3299,7 +3344,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -3334,7 +3379,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
@@ -3369,7 +3414,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
@@ -3404,7 +3449,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -3439,7 +3484,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
@@ -3474,7 +3519,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
@@ -3509,7 +3554,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
@@ -3544,7 +3589,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -3579,7 +3624,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
@@ -3614,7 +3659,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>3</v>
       </c>
@@ -3649,7 +3694,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
@@ -3681,7 +3726,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -3716,19 +3761,19 @@
         <v>326</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
     </row>
   </sheetData>
@@ -3738,21 +3783,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>51</v>
       </c>
@@ -3763,7 +3808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>53</v>
       </c>
@@ -3774,7 +3819,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>55</v>
       </c>
@@ -3785,7 +3830,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>57</v>
       </c>
@@ -3796,7 +3841,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>59</v>
       </c>
@@ -3807,7 +3852,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>61</v>
       </c>
@@ -3818,7 +3863,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>63</v>
       </c>
@@ -3829,7 +3874,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>65</v>
       </c>
@@ -3840,7 +3885,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>67</v>
       </c>
@@ -3851,7 +3896,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>69</v>
       </c>
@@ -3862,7 +3907,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>71</v>
       </c>
@@ -3873,7 +3918,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>73</v>
       </c>
@@ -3884,7 +3929,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>75</v>
       </c>
@@ -3895,7 +3940,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>77</v>
       </c>
@@ -3906,7 +3951,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>79</v>
       </c>
@@ -3917,7 +3962,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>81</v>
       </c>
@@ -3928,7 +3973,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>83</v>
       </c>
@@ -3939,7 +3984,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>85</v>
       </c>
@@ -3950,7 +3995,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>87</v>
       </c>
@@ -3961,7 +4006,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>89</v>
       </c>
@@ -3972,7 +4017,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>91</v>
       </c>
@@ -3983,7 +4028,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>92</v>
       </c>
@@ -3994,7 +4039,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>97</v>
       </c>
@@ -4005,7 +4050,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>95</v>
       </c>

</xml_diff>

<commit_message>
BCA is still incomplete
</commit_message>
<xml_diff>
--- a/Time-table.xlsx
+++ b/Time-table.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6E25FA-6635-472D-A596-60C1F75E2C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Rooms" sheetId="1" r:id="rId1"/>
     <sheet name="Timetable" sheetId="2" r:id="rId2"/>
     <sheet name="Odd_sem" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
+    <sheet name="BCA" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="259">
   <si>
     <t>Class</t>
   </si>
@@ -702,14 +702,107 @@
     <t>Kartik Konar, Sulaxan</t>
   </si>
   <si>
-    <t>Shilpa Marathe B</t>
+    <t>BCA</t>
+  </si>
+  <si>
+    <t>BCA 153</t>
+  </si>
+  <si>
+    <t>Mrs.Nikita Pagar</t>
+  </si>
+  <si>
+    <t>BCA 151</t>
+  </si>
+  <si>
+    <t>Relational Database Management System</t>
+  </si>
+  <si>
+    <t>Mrs.Maya Pisal</t>
+  </si>
+  <si>
+    <t>BCA 152</t>
+  </si>
+  <si>
+    <t>Object oriented concepts and Programming (Java)</t>
+  </si>
+  <si>
+    <t>Mr.Nikhil Soniminde</t>
+  </si>
+  <si>
+    <t>BCA 154</t>
+  </si>
+  <si>
+    <t>Design Thinking</t>
+  </si>
+  <si>
+    <t>Mr.Akash Dange</t>
+  </si>
+  <si>
+    <t>BCA 155</t>
+  </si>
+  <si>
+    <t>Skill Development</t>
+  </si>
+  <si>
+    <t>Ms.Vahida Pathan</t>
+  </si>
+  <si>
+    <t>Mrs. Prachi Soniminde</t>
+  </si>
+  <si>
+    <t>Varshita</t>
+  </si>
+  <si>
+    <t>Mr.Anil Narasipuram</t>
+  </si>
+  <si>
+    <t>BCA 255</t>
+  </si>
+  <si>
+    <t>Environmental Studies</t>
+  </si>
+  <si>
+    <t>Ms. Prachi Soniminde</t>
+  </si>
+  <si>
+    <t>BCA 251</t>
+  </si>
+  <si>
+    <t>Introduction to Cloud Computing</t>
+  </si>
+  <si>
+    <t>BCA 253</t>
+  </si>
+  <si>
+    <t>Operating Systems</t>
+  </si>
+  <si>
+    <t>Mrs.Heena Bhatia</t>
+  </si>
+  <si>
+    <t>BCA 252</t>
+  </si>
+  <si>
+    <t>Introduction to Mobile Computing</t>
+  </si>
+  <si>
+    <t>Ms.Pallavi Shimpi</t>
+  </si>
+  <si>
+    <t>BCA 204</t>
+  </si>
+  <si>
+    <t>Software Engineering</t>
+  </si>
+  <si>
+    <t>Ms.Suvarna Karankal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -744,8 +837,27 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF00000A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -776,7 +888,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -814,6 +926,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -907,23 +1022,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -959,23 +1057,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1151,17 +1232,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>216</v>
       </c>
@@ -1172,7 +1253,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>306</v>
       </c>
@@ -1183,7 +1264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>313</v>
       </c>
@@ -1194,7 +1275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>341</v>
       </c>
@@ -1205,7 +1286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>328</v>
       </c>
@@ -1216,7 +1297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>329</v>
       </c>
@@ -1227,7 +1308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>330</v>
       </c>
@@ -1238,7 +1319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>331</v>
       </c>
@@ -1249,7 +1330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>332</v>
       </c>
@@ -1260,7 +1341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>333</v>
       </c>
@@ -1271,7 +1352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>334</v>
       </c>
@@ -1282,7 +1363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>336</v>
       </c>
@@ -1293,7 +1374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>338</v>
       </c>
@@ -1304,7 +1385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>339</v>
       </c>
@@ -1315,7 +1396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>337</v>
       </c>
@@ -1326,7 +1407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>305</v>
       </c>
@@ -1337,7 +1418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>314</v>
       </c>
@@ -1348,7 +1429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>335</v>
       </c>
@@ -1359,7 +1440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>406</v>
       </c>
@@ -1370,7 +1451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>409</v>
       </c>
@@ -1381,7 +1462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>430</v>
       </c>
@@ -1392,7 +1473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>432</v>
       </c>
@@ -1403,7 +1484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>440</v>
       </c>
@@ -1414,7 +1495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>431</v>
       </c>
@@ -1425,7 +1506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>405</v>
       </c>
@@ -1436,7 +1517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>410</v>
       </c>
@@ -1447,7 +1528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>433</v>
       </c>
@@ -1458,7 +1539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>434</v>
       </c>
@@ -1469,7 +1550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>435</v>
       </c>
@@ -1480,7 +1561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>436</v>
       </c>
@@ -1491,7 +1572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>437</v>
       </c>
@@ -1502,7 +1583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>438</v>
       </c>
@@ -1513,7 +1594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>325</v>
       </c>
@@ -1524,7 +1605,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>324</v>
       </c>
@@ -1535,7 +1616,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>353</v>
       </c>
@@ -1546,7 +1627,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>322</v>
       </c>
@@ -1557,7 +1638,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>346</v>
       </c>
@@ -1568,7 +1649,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>326</v>
       </c>
@@ -1579,7 +1660,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>327</v>
       </c>
@@ -1590,7 +1671,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>356</v>
       </c>
@@ -1601,7 +1682,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>354</v>
       </c>
@@ -1612,7 +1693,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>421</v>
       </c>
@@ -1623,7 +1704,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>420</v>
       </c>
@@ -1634,7 +1715,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>413</v>
       </c>
@@ -1645,7 +1726,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>453</v>
       </c>
@@ -1656,7 +1737,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>445</v>
       </c>
@@ -1667,7 +1748,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>446</v>
       </c>
@@ -1678,7 +1759,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>449</v>
       </c>
@@ -1689,7 +1770,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>407</v>
       </c>
@@ -1700,7 +1781,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>408</v>
       </c>
@@ -1711,7 +1792,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>450</v>
       </c>
@@ -1729,27 +1810,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="6" width="22.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="6" width="22.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.109375" customWidth="1"/>
+    <col min="14" max="14" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>214</v>
       </c>
@@ -1793,7 +1874,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1807,7 +1888,7 @@
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G2" s="1">
@@ -1829,7 +1910,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1843,7 +1924,7 @@
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="1" t="s">
         <v>43</v>
       </c>
       <c r="G3" s="1">
@@ -1865,7 +1946,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1879,7 +1960,7 @@
       <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="1" t="s">
         <v>44</v>
       </c>
       <c r="G4" s="1">
@@ -1901,7 +1982,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1915,7 +1996,7 @@
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G5" s="1">
@@ -1935,7 +2016,7 @@
       </c>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1949,7 +2030,7 @@
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="1" t="s">
         <v>119</v>
       </c>
       <c r="G6" s="1">
@@ -1969,7 +2050,7 @@
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1983,7 +2064,7 @@
       <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="1" t="s">
         <v>47</v>
       </c>
       <c r="G7" s="1">
@@ -2005,7 +2086,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -2019,7 +2100,7 @@
       <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="1" t="s">
         <v>48</v>
       </c>
       <c r="G8" s="1">
@@ -2039,7 +2120,7 @@
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -2053,7 +2134,7 @@
       <c r="E9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="1" t="s">
         <v>49</v>
       </c>
       <c r="G9" s="1">
@@ -2075,7 +2156,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -2089,7 +2170,7 @@
       <c r="E10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G10" s="1">
@@ -2111,7 +2192,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -2125,7 +2206,7 @@
       <c r="E11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="1" t="s">
         <v>43</v>
       </c>
       <c r="G11" s="1">
@@ -2147,7 +2228,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -2161,7 +2242,7 @@
       <c r="E12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="1" t="s">
         <v>119</v>
       </c>
       <c r="G12" s="1">
@@ -2181,7 +2262,7 @@
       </c>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -2195,7 +2276,7 @@
       <c r="E13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="1" t="s">
         <v>119</v>
       </c>
       <c r="G13" s="1">
@@ -2215,7 +2296,7 @@
       </c>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -2231,7 +2312,7 @@
       <c r="E14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="11" t="s">
         <v>112</v>
       </c>
       <c r="G14" s="1">
@@ -2259,7 +2340,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -2275,7 +2356,7 @@
       <c r="E15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="11" t="s">
         <v>107</v>
       </c>
       <c r="G15" s="1">
@@ -2303,7 +2384,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -2319,7 +2400,7 @@
       <c r="E16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="11" t="s">
         <v>108</v>
       </c>
       <c r="G16" s="1">
@@ -2344,7 +2425,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -2360,7 +2441,7 @@
       <c r="E17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="11" t="s">
         <v>109</v>
       </c>
       <c r="G17" s="1">
@@ -2385,7 +2466,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -2401,7 +2482,7 @@
       <c r="E18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="11" t="s">
         <v>110</v>
       </c>
       <c r="G18" s="1">
@@ -2426,7 +2507,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -2442,7 +2523,7 @@
       <c r="E19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F19" s="11" t="s">
         <v>111</v>
       </c>
       <c r="G19" s="1">
@@ -2467,7 +2548,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -2483,8 +2564,8 @@
       <c r="E20" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F20" s="16" t="s">
-        <v>227</v>
+      <c r="F20" s="11" t="s">
+        <v>111</v>
       </c>
       <c r="G20" s="1">
         <v>6</v>
@@ -2508,7 +2589,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
@@ -2524,7 +2605,7 @@
       <c r="E21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="11" t="s">
         <v>107</v>
       </c>
       <c r="G21" s="1">
@@ -2549,7 +2630,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
@@ -2565,7 +2646,7 @@
       <c r="E22" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="11" t="s">
         <v>110</v>
       </c>
       <c r="G22" s="1">
@@ -2590,7 +2671,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -2606,7 +2687,7 @@
       <c r="E23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="11" t="s">
         <v>119</v>
       </c>
       <c r="G23" s="1">
@@ -2631,7 +2712,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
@@ -2647,7 +2728,7 @@
       <c r="E24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="11" t="s">
         <v>119</v>
       </c>
       <c r="G24" s="1">
@@ -2670,7 +2751,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
@@ -2716,28 +2797,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="41.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="38.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="41.109375" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" customWidth="1"/>
+    <col min="6" max="6" width="38.5546875" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" customWidth="1"/>
+    <col min="14" max="14" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>214</v>
       </c>
@@ -2781,7 +2862,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2810,7 +2891,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2836,7 +2917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2862,7 +2943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2891,7 +2972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2917,7 +2998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -2942,8 +3023,14 @@
       <c r="I7">
         <v>1</v>
       </c>
+      <c r="J7">
+        <v>120</v>
+      </c>
       <c r="K7">
         <v>2</v>
+      </c>
+      <c r="L7">
+        <v>60</v>
       </c>
       <c r="M7">
         <v>430</v>
@@ -2952,7 +3039,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -2977,8 +3064,14 @@
       <c r="I8">
         <v>1</v>
       </c>
+      <c r="J8">
+        <v>120</v>
+      </c>
       <c r="K8">
         <v>2</v>
+      </c>
+      <c r="L8">
+        <v>60</v>
       </c>
       <c r="M8">
         <v>430</v>
@@ -2987,7 +3080,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -3009,6 +3102,9 @@
       <c r="I9">
         <v>0</v>
       </c>
+      <c r="J9">
+        <v>120</v>
+      </c>
       <c r="K9">
         <v>0</v>
       </c>
@@ -3016,7 +3112,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -3041,8 +3137,14 @@
       <c r="I10">
         <v>1</v>
       </c>
+      <c r="J10">
+        <v>120</v>
+      </c>
       <c r="K10">
         <v>2</v>
+      </c>
+      <c r="L10">
+        <v>60</v>
       </c>
       <c r="M10">
         <v>430</v>
@@ -3051,7 +3153,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -3073,6 +3175,9 @@
       <c r="I11">
         <v>0</v>
       </c>
+      <c r="J11">
+        <v>120</v>
+      </c>
       <c r="K11">
         <v>0</v>
       </c>
@@ -3080,7 +3185,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -3105,6 +3210,9 @@
       <c r="I12">
         <v>0</v>
       </c>
+      <c r="J12">
+        <v>120</v>
+      </c>
       <c r="K12">
         <v>0</v>
       </c>
@@ -3112,7 +3220,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -3137,14 +3245,23 @@
       <c r="I13">
         <v>1</v>
       </c>
+      <c r="J13">
+        <v>120</v>
+      </c>
       <c r="K13">
         <v>2</v>
+      </c>
+      <c r="L13">
+        <v>60</v>
       </c>
       <c r="M13">
         <v>432</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -3166,6 +3283,9 @@
       <c r="I14">
         <v>0</v>
       </c>
+      <c r="J14">
+        <v>120</v>
+      </c>
       <c r="K14">
         <v>0</v>
       </c>
@@ -3173,7 +3293,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -3198,14 +3318,23 @@
       <c r="I15">
         <v>1</v>
       </c>
+      <c r="J15">
+        <v>120</v>
+      </c>
       <c r="K15">
         <v>2</v>
+      </c>
+      <c r="L15">
+        <v>60</v>
       </c>
       <c r="M15">
         <v>432</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>3</v>
       </c>
@@ -3233,16 +3362,23 @@
       <c r="I16" s="13">
         <v>1</v>
       </c>
-      <c r="J16" s="13"/>
+      <c r="J16" s="13">
+        <v>120</v>
+      </c>
       <c r="K16" s="13">
         <v>2</v>
       </c>
-      <c r="L16" s="13"/>
+      <c r="L16">
+        <v>60</v>
+      </c>
       <c r="M16">
         <v>432</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="13">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -3270,14 +3406,23 @@
       <c r="I17">
         <v>1</v>
       </c>
+      <c r="J17">
+        <v>120</v>
+      </c>
       <c r="K17">
         <v>2</v>
+      </c>
+      <c r="L17">
+        <v>60</v>
       </c>
       <c r="M17">
         <v>432</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -3305,14 +3450,23 @@
       <c r="I18">
         <v>1</v>
       </c>
+      <c r="J18">
+        <v>120</v>
+      </c>
       <c r="K18">
         <v>2</v>
+      </c>
+      <c r="L18">
+        <v>60</v>
       </c>
       <c r="M18">
         <v>432</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -3337,14 +3491,23 @@
       <c r="I19">
         <v>1</v>
       </c>
+      <c r="J19">
+        <v>60</v>
+      </c>
       <c r="K19">
         <v>2</v>
       </c>
+      <c r="L19">
+        <v>60</v>
+      </c>
       <c r="M19">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+      <c r="N19">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -3372,14 +3535,23 @@
       <c r="I20">
         <v>1</v>
       </c>
+      <c r="J20">
+        <v>120</v>
+      </c>
       <c r="K20">
         <v>2</v>
+      </c>
+      <c r="L20">
+        <v>60</v>
       </c>
       <c r="M20">
         <v>440</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
@@ -3407,14 +3579,23 @@
       <c r="I21">
         <v>1</v>
       </c>
+      <c r="J21">
+        <v>120</v>
+      </c>
       <c r="K21">
         <v>2</v>
+      </c>
+      <c r="L21">
+        <v>60</v>
       </c>
       <c r="M21">
         <v>440</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
@@ -3442,14 +3623,23 @@
       <c r="I22">
         <v>1</v>
       </c>
+      <c r="J22">
+        <v>120</v>
+      </c>
       <c r="K22">
         <v>2</v>
+      </c>
+      <c r="L22">
+        <v>60</v>
       </c>
       <c r="M22">
         <v>440</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -3477,14 +3667,20 @@
       <c r="I23">
         <v>1</v>
       </c>
+      <c r="J23">
+        <v>60</v>
+      </c>
       <c r="K23">
         <v>2</v>
       </c>
+      <c r="L23">
+        <v>60</v>
+      </c>
       <c r="M23">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
@@ -3512,14 +3708,23 @@
       <c r="I24">
         <v>1</v>
       </c>
+      <c r="J24">
+        <v>120</v>
+      </c>
       <c r="K24">
         <v>2</v>
+      </c>
+      <c r="L24">
+        <v>60</v>
       </c>
       <c r="M24">
         <v>440</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
@@ -3547,14 +3752,20 @@
       <c r="I25">
         <v>1</v>
       </c>
+      <c r="J25">
+        <v>60</v>
+      </c>
       <c r="K25">
         <v>2</v>
       </c>
+      <c r="L25">
+        <v>60</v>
+      </c>
       <c r="M25">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
@@ -3582,14 +3793,23 @@
       <c r="I26">
         <v>1</v>
       </c>
+      <c r="J26">
+        <v>60</v>
+      </c>
       <c r="K26">
         <v>2</v>
       </c>
+      <c r="L26">
+        <v>60</v>
+      </c>
       <c r="M26">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>438</v>
+      </c>
+      <c r="N26">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -3617,14 +3837,23 @@
       <c r="I27">
         <v>1</v>
       </c>
+      <c r="J27">
+        <v>60</v>
+      </c>
       <c r="K27">
         <v>2</v>
       </c>
+      <c r="L27">
+        <v>60</v>
+      </c>
       <c r="M27">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+        <v>438</v>
+      </c>
+      <c r="N27">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
@@ -3652,14 +3881,23 @@
       <c r="I28">
         <v>1</v>
       </c>
+      <c r="J28">
+        <v>60</v>
+      </c>
       <c r="K28">
         <v>2</v>
       </c>
+      <c r="L28">
+        <v>60</v>
+      </c>
       <c r="M28">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+        <v>438</v>
+      </c>
+      <c r="N28">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>3</v>
       </c>
@@ -3687,14 +3925,23 @@
       <c r="I29">
         <v>1</v>
       </c>
+      <c r="J29">
+        <v>60</v>
+      </c>
       <c r="K29">
         <v>2</v>
       </c>
+      <c r="L29">
+        <v>60</v>
+      </c>
       <c r="M29">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+      <c r="N29">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
@@ -3719,14 +3966,23 @@
       <c r="I30">
         <v>1</v>
       </c>
+      <c r="J30">
+        <v>60</v>
+      </c>
       <c r="K30">
         <v>2</v>
       </c>
+      <c r="L30">
+        <v>60</v>
+      </c>
       <c r="M30">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+      <c r="N30">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -3754,26 +4010,35 @@
       <c r="I31">
         <v>1</v>
       </c>
+      <c r="J31">
+        <v>60</v>
+      </c>
       <c r="K31">
         <v>2</v>
       </c>
+      <c r="L31">
+        <v>60</v>
+      </c>
       <c r="M31">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+      <c r="N31">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
     </row>
   </sheetData>
@@ -3783,21 +4048,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="11.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>51</v>
       </c>
@@ -3808,7 +4073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>53</v>
       </c>
@@ -3819,7 +4084,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>55</v>
       </c>
@@ -3830,7 +4095,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>57</v>
       </c>
@@ -3841,7 +4106,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>59</v>
       </c>
@@ -3852,7 +4117,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>61</v>
       </c>
@@ -3863,7 +4128,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>63</v>
       </c>
@@ -3874,7 +4139,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>65</v>
       </c>
@@ -3885,7 +4150,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>67</v>
       </c>
@@ -3896,7 +4161,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>69</v>
       </c>
@@ -3907,7 +4172,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>71</v>
       </c>
@@ -3918,7 +4183,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>73</v>
       </c>
@@ -3929,7 +4194,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>75</v>
       </c>
@@ -3940,7 +4205,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>77</v>
       </c>
@@ -3951,7 +4216,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>79</v>
       </c>
@@ -3962,7 +4227,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>81</v>
       </c>
@@ -3973,7 +4238,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>83</v>
       </c>
@@ -3984,7 +4249,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>85</v>
       </c>
@@ -3995,7 +4260,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>87</v>
       </c>
@@ -4006,7 +4271,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>89</v>
       </c>
@@ -4017,7 +4282,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>91</v>
       </c>
@@ -4028,7 +4293,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>92</v>
       </c>
@@ -4039,7 +4304,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>97</v>
       </c>
@@ -4050,7 +4315,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>95</v>
       </c>
@@ -4059,6 +4324,534 @@
       </c>
       <c r="C24" s="4">
         <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="42.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="14.88671875" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" customWidth="1"/>
+    <col min="14" max="14" width="14.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>120</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2">
+        <v>60</v>
+      </c>
+      <c r="M2">
+        <v>409</v>
+      </c>
+      <c r="N2">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>120</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>60</v>
+      </c>
+      <c r="M3">
+        <v>409</v>
+      </c>
+      <c r="N3">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>120</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>60</v>
+      </c>
+      <c r="M4">
+        <v>409</v>
+      </c>
+      <c r="N4">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>120</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>60</v>
+      </c>
+      <c r="M5">
+        <v>409</v>
+      </c>
+      <c r="N5">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>120</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>60</v>
+      </c>
+      <c r="M6">
+        <v>409</v>
+      </c>
+      <c r="N6">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>120</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>60</v>
+      </c>
+      <c r="M7">
+        <v>409</v>
+      </c>
+      <c r="N7">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>120</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <v>60</v>
+      </c>
+      <c r="M8">
+        <v>409</v>
+      </c>
+      <c r="N8">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>227</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>120</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>60</v>
+      </c>
+      <c r="M9">
+        <v>409</v>
+      </c>
+      <c r="N9">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>227</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>120</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>60</v>
+      </c>
+      <c r="M10">
+        <v>409</v>
+      </c>
+      <c r="N10">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>227</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>120</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <v>60</v>
+      </c>
+      <c r="M11">
+        <v>409</v>
+      </c>
+      <c r="N11">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>227</v>
+      </c>
+      <c r="J12">
+        <v>120</v>
+      </c>
+      <c r="L12">
+        <v>60</v>
+      </c>
+      <c r="M12">
+        <v>409</v>
+      </c>
+      <c r="N12">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The last chicken day
</commit_message>
<xml_diff>
--- a/Time-table.xlsx
+++ b/Time-table.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8209EC16-C9A1-4660-8728-6B9655BA2066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rooms" sheetId="1" r:id="rId1"/>
     <sheet name="Timetable" sheetId="2" r:id="rId2"/>
     <sheet name="Odd_sem" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
-    <sheet name="BCA" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="227">
   <si>
     <t>Class</t>
   </si>
@@ -38,12 +38,6 @@
     <t>Dr.Yogesh Sariya</t>
   </si>
   <si>
-    <t>Dr.Rajshekar</t>
-  </si>
-  <si>
-    <t>Dr.Anju Chaurasia</t>
-  </si>
-  <si>
     <t>Dr.Shashi Singh</t>
   </si>
   <si>
@@ -80,18 +74,6 @@
     <t>Amit Kumar Om</t>
   </si>
   <si>
-    <t>DS</t>
-  </si>
-  <si>
-    <t>DLD</t>
-  </si>
-  <si>
-    <t>DTFW</t>
-  </si>
-  <si>
-    <t>ACM II</t>
-  </si>
-  <si>
     <t>HP</t>
   </si>
   <si>
@@ -155,9 +137,6 @@
     <t>Rajkumar</t>
   </si>
   <si>
-    <t>Varsha Sambaje</t>
-  </si>
-  <si>
     <t>ICS</t>
   </si>
   <si>
@@ -359,25 +338,13 @@
     <t>Shrikant M</t>
   </si>
   <si>
-    <t>RHPC</t>
-  </si>
-  <si>
     <t>Faculty</t>
   </si>
   <si>
     <t>Lab_Capacity</t>
   </si>
   <si>
-    <t>Prof. Vinayak Sathe B</t>
-  </si>
-  <si>
-    <t>Prof. Vinayak Sathe C</t>
-  </si>
-  <si>
     <t>DS (DSC602)</t>
-  </si>
-  <si>
-    <t>None</t>
   </si>
   <si>
     <t>CSE101</t>
@@ -702,107 +669,44 @@
     <t>Kartik Konar, Sulaxan</t>
   </si>
   <si>
-    <t>BCA</t>
-  </si>
-  <si>
-    <t>BCA 153</t>
-  </si>
-  <si>
-    <t>Mrs.Nikita Pagar</t>
-  </si>
-  <si>
-    <t>BCA 151</t>
-  </si>
-  <si>
-    <t>Relational Database Management System</t>
-  </si>
-  <si>
-    <t>Mrs.Maya Pisal</t>
-  </si>
-  <si>
-    <t>BCA 152</t>
-  </si>
-  <si>
-    <t>Object oriented concepts and Programming (Java)</t>
-  </si>
-  <si>
-    <t>Mr.Nikhil Soniminde</t>
-  </si>
-  <si>
-    <t>BCA 154</t>
-  </si>
-  <si>
-    <t>Design Thinking</t>
-  </si>
-  <si>
-    <t>Mr.Akash Dange</t>
-  </si>
-  <si>
-    <t>BCA 155</t>
-  </si>
-  <si>
-    <t>Skill Development</t>
-  </si>
-  <si>
-    <t>Ms.Vahida Pathan</t>
-  </si>
-  <si>
-    <t>Mrs. Prachi Soniminde</t>
-  </si>
-  <si>
-    <t>Varshita</t>
-  </si>
-  <si>
-    <t>Mr.Anil Narasipuram</t>
-  </si>
-  <si>
-    <t>BCA 255</t>
-  </si>
-  <si>
-    <t>Environmental Studies</t>
-  </si>
-  <si>
-    <t>Ms. Prachi Soniminde</t>
-  </si>
-  <si>
-    <t>BCA 251</t>
-  </si>
-  <si>
-    <t>Introduction to Cloud Computing</t>
-  </si>
-  <si>
-    <t>BCA 253</t>
-  </si>
-  <si>
-    <t>Operating Systems</t>
-  </si>
-  <si>
-    <t>Mrs.Heena Bhatia</t>
-  </si>
-  <si>
-    <t>BCA 252</t>
-  </si>
-  <si>
-    <t>Introduction to Mobile Computing</t>
-  </si>
-  <si>
-    <t>Ms.Pallavi Shimpi</t>
-  </si>
-  <si>
-    <t>BCA 204</t>
-  </si>
-  <si>
-    <t>Software Engineering</t>
-  </si>
-  <si>
-    <t>Ms.Suvarna Karankal</t>
+    <t>AI (AIM602), ROBO (ROB602)</t>
+  </si>
+  <si>
+    <t>OEL1</t>
+  </si>
+  <si>
+    <t>OEL2</t>
+  </si>
+  <si>
+    <t>OEL3</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>DLD</t>
+  </si>
+  <si>
+    <t>DTFW</t>
+  </si>
+  <si>
+    <t>Dr.Rajshekar</t>
+  </si>
+  <si>
+    <t>ACM II</t>
+  </si>
+  <si>
+    <t>Dr.Anju Chaurasia</t>
+  </si>
+  <si>
+    <t>Varsha Sambaje</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -837,29 +741,16 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="8"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF00000A"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -888,7 +779,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -915,7 +806,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -926,9 +816,11 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1022,6 +914,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1057,6 +966,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1232,28 +1158,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>306</v>
       </c>
@@ -1264,7 +1192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>313</v>
       </c>
@@ -1275,7 +1203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>341</v>
       </c>
@@ -1286,7 +1214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>328</v>
       </c>
@@ -1297,7 +1225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>329</v>
       </c>
@@ -1308,7 +1236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>330</v>
       </c>
@@ -1319,7 +1247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>331</v>
       </c>
@@ -1330,7 +1258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>332</v>
       </c>
@@ -1341,7 +1269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>333</v>
       </c>
@@ -1352,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>334</v>
       </c>
@@ -1363,7 +1291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>336</v>
       </c>
@@ -1374,7 +1302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>338</v>
       </c>
@@ -1385,7 +1313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>339</v>
       </c>
@@ -1396,7 +1324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>337</v>
       </c>
@@ -1407,7 +1335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>305</v>
       </c>
@@ -1418,7 +1346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>314</v>
       </c>
@@ -1429,7 +1357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>335</v>
       </c>
@@ -1440,7 +1368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>406</v>
       </c>
@@ -1451,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>409</v>
       </c>
@@ -1462,7 +1390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>430</v>
       </c>
@@ -1473,7 +1401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>432</v>
       </c>
@@ -1484,7 +1412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>440</v>
       </c>
@@ -1495,7 +1423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>431</v>
       </c>
@@ -1506,7 +1434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>405</v>
       </c>
@@ -1517,7 +1445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>410</v>
       </c>
@@ -1528,7 +1456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>433</v>
       </c>
@@ -1539,7 +1467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>434</v>
       </c>
@@ -1550,7 +1478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>435</v>
       </c>
@@ -1561,7 +1489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>436</v>
       </c>
@@ -1572,7 +1500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>437</v>
       </c>
@@ -1583,7 +1511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>438</v>
       </c>
@@ -1594,7 +1522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>325</v>
       </c>
@@ -1602,10 +1530,10 @@
         <v>60</v>
       </c>
       <c r="C33" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>324</v>
       </c>
@@ -1613,10 +1541,10 @@
         <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>353</v>
       </c>
@@ -1624,10 +1552,10 @@
         <v>60</v>
       </c>
       <c r="C35" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>322</v>
       </c>
@@ -1635,10 +1563,10 @@
         <v>60</v>
       </c>
       <c r="C36" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>346</v>
       </c>
@@ -1646,10 +1574,10 @@
         <v>60</v>
       </c>
       <c r="C37" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>326</v>
       </c>
@@ -1657,10 +1585,10 @@
         <v>60</v>
       </c>
       <c r="C38" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>327</v>
       </c>
@@ -1668,10 +1596,10 @@
         <v>60</v>
       </c>
       <c r="C39" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>356</v>
       </c>
@@ -1679,10 +1607,10 @@
         <v>30</v>
       </c>
       <c r="C40" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>354</v>
       </c>
@@ -1690,10 +1618,10 @@
         <v>30</v>
       </c>
       <c r="C41" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>421</v>
       </c>
@@ -1701,10 +1629,10 @@
         <v>60</v>
       </c>
       <c r="C42" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>420</v>
       </c>
@@ -1712,10 +1640,10 @@
         <v>60</v>
       </c>
       <c r="C43" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>413</v>
       </c>
@@ -1723,10 +1651,10 @@
         <v>60</v>
       </c>
       <c r="C44" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>453</v>
       </c>
@@ -1734,10 +1662,10 @@
         <v>60</v>
       </c>
       <c r="C45" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>445</v>
       </c>
@@ -1745,10 +1673,10 @@
         <v>60</v>
       </c>
       <c r="C46" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>446</v>
       </c>
@@ -1756,10 +1684,10 @@
         <v>60</v>
       </c>
       <c r="C47" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>449</v>
       </c>
@@ -1767,10 +1695,10 @@
         <v>60</v>
       </c>
       <c r="C48" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>407</v>
       </c>
@@ -1778,10 +1706,10 @@
         <v>60</v>
       </c>
       <c r="C49" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>408</v>
       </c>
@@ -1789,18 +1717,18 @@
         <v>60</v>
       </c>
       <c r="C50" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>450</v>
       </c>
       <c r="B51">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C51" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -1810,298 +1738,308 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="6" width="22.5546875" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.109375" customWidth="1"/>
-    <col min="14" max="14" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="6" width="22.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="1">
-        <v>2</v>
-      </c>
-      <c r="H2" s="1">
-        <v>3</v>
-      </c>
-      <c r="I2" s="1">
-        <v>1</v>
-      </c>
-      <c r="J2" s="1">
-        <v>120</v>
-      </c>
-      <c r="K2" s="1">
-        <v>2</v>
-      </c>
-      <c r="L2" s="1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="F2" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="17">
+        <v>2</v>
+      </c>
+      <c r="H2" s="17">
+        <v>3</v>
+      </c>
+      <c r="I2" s="17">
+        <v>1</v>
+      </c>
+      <c r="J2" s="17">
+        <v>120</v>
+      </c>
+      <c r="K2" s="17">
+        <v>2</v>
+      </c>
+      <c r="L2" s="17">
+        <v>60</v>
+      </c>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="1">
-        <v>2</v>
-      </c>
-      <c r="H3" s="1">
-        <v>3</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1</v>
-      </c>
-      <c r="J3" s="1">
-        <v>120</v>
-      </c>
-      <c r="K3" s="1">
-        <v>2</v>
-      </c>
-      <c r="L3" s="1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="F3" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="17">
+        <v>2</v>
+      </c>
+      <c r="H3" s="17">
+        <v>3</v>
+      </c>
+      <c r="I3" s="17">
+        <v>1</v>
+      </c>
+      <c r="J3" s="17">
+        <v>120</v>
+      </c>
+      <c r="K3" s="17">
+        <v>2</v>
+      </c>
+      <c r="L3" s="17">
+        <v>60</v>
+      </c>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="17">
+        <v>2</v>
+      </c>
+      <c r="H4" s="17">
+        <v>3</v>
+      </c>
+      <c r="I4" s="17">
+        <v>0</v>
+      </c>
+      <c r="J4" s="17">
+        <v>120</v>
+      </c>
+      <c r="K4" s="17">
+        <v>2</v>
+      </c>
+      <c r="L4" s="17">
+        <v>60</v>
+      </c>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="G5" s="17">
+        <v>2</v>
+      </c>
+      <c r="H5" s="17">
+        <v>3</v>
+      </c>
+      <c r="I5" s="17">
+        <v>1</v>
+      </c>
+      <c r="J5" s="17">
+        <v>120</v>
+      </c>
+      <c r="K5" s="17">
+        <v>0</v>
+      </c>
+      <c r="L5" s="17"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+    </row>
+    <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" s="1">
-        <v>2</v>
-      </c>
-      <c r="H4" s="1">
-        <v>3</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>120</v>
-      </c>
-      <c r="K4" s="1">
-        <v>2</v>
-      </c>
-      <c r="L4" s="1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="F6" s="17"/>
+      <c r="G6" s="17">
+        <v>2</v>
+      </c>
+      <c r="H6" s="17">
+        <v>3</v>
+      </c>
+      <c r="I6" s="17">
+        <v>0</v>
+      </c>
+      <c r="J6" s="17">
+        <v>120</v>
+      </c>
+      <c r="K6" s="17">
+        <v>0</v>
+      </c>
+      <c r="L6" s="17"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="1">
-        <v>2</v>
-      </c>
-      <c r="H5" s="1">
-        <v>3</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1">
-        <v>120</v>
-      </c>
-      <c r="K5" s="1">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G6" s="1">
-        <v>2</v>
-      </c>
-      <c r="H6" s="1">
-        <v>3</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1">
-        <v>120</v>
-      </c>
-      <c r="K6" s="1">
-        <v>0</v>
-      </c>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="17">
+        <v>2</v>
+      </c>
+      <c r="H7" s="17">
+        <v>3</v>
+      </c>
+      <c r="I7" s="17">
+        <v>1</v>
+      </c>
+      <c r="J7" s="17">
+        <v>120</v>
+      </c>
+      <c r="K7" s="17">
+        <v>2</v>
+      </c>
+      <c r="L7" s="17">
+        <v>60</v>
+      </c>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="1">
-        <v>2</v>
-      </c>
-      <c r="H7" s="1">
-        <v>3</v>
-      </c>
-      <c r="I7" s="1">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1">
-        <v>120</v>
-      </c>
-      <c r="K7" s="1">
-        <v>2</v>
-      </c>
-      <c r="L7" s="1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>48</v>
+        <v>8</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="G8" s="1">
         <v>4</v>
@@ -2119,23 +2057,24 @@
         <v>0</v>
       </c>
       <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M8" s="19"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>49</v>
+        <v>9</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>42</v>
       </c>
       <c r="G9" s="1">
         <v>4</v>
@@ -2155,23 +2094,24 @@
       <c r="L9" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M9" s="19"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>50</v>
+        <v>10</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>43</v>
       </c>
       <c r="G10" s="1">
         <v>4</v>
@@ -2191,23 +2131,24 @@
       <c r="L10" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M10" s="19"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>43</v>
+        <v>11</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>37</v>
       </c>
       <c r="G11" s="1">
         <v>4</v>
@@ -2227,24 +2168,23 @@
       <c r="L11" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M11" s="19"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>119</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F12" s="15"/>
       <c r="G12" s="1">
         <v>4</v>
       </c>
@@ -2261,24 +2201,23 @@
         <v>0</v>
       </c>
       <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M12" s="19"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>119</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F13" s="15"/>
       <c r="G13" s="1">
         <v>4</v>
       </c>
@@ -2295,25 +2234,26 @@
         <v>0</v>
       </c>
       <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="15" t="s">
         <v>105</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>112</v>
       </c>
       <c r="G14" s="1">
         <v>6</v>
@@ -2333,31 +2273,27 @@
       <c r="L14" s="1">
         <v>60</v>
       </c>
-      <c r="M14" s="1">
-        <v>440</v>
-      </c>
-      <c r="N14" s="1">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M14" s="20"/>
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>107</v>
+        <v>13</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>100</v>
       </c>
       <c r="G15" s="1">
         <v>6</v>
@@ -2377,31 +2313,26 @@
       <c r="L15" s="1">
         <v>60</v>
       </c>
-      <c r="M15" s="1">
-        <v>440</v>
-      </c>
-      <c r="N15" s="1">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M15" s="20"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>108</v>
+      <c r="F16" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="G16" s="1">
         <v>6</v>
@@ -2421,28 +2352,26 @@
       <c r="L16" s="1">
         <v>60</v>
       </c>
-      <c r="M16" s="1">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M16" s="20"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>109</v>
+        <v>14</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>102</v>
       </c>
       <c r="G17" s="1">
         <v>6</v>
@@ -2462,28 +2391,26 @@
       <c r="L17" s="1">
         <v>60</v>
       </c>
-      <c r="M17" s="1">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M17" s="20"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>110</v>
+        <v>10</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>103</v>
       </c>
       <c r="G18" s="1">
         <v>6</v>
@@ -2503,28 +2430,26 @@
       <c r="L18" s="1">
         <v>60</v>
       </c>
-      <c r="M18" s="1">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M18" s="20"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>87</v>
+        <v>216</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="15" t="s">
         <v>104</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="G19" s="1">
         <v>6</v>
@@ -2536,7 +2461,7 @@
         <v>1</v>
       </c>
       <c r="J19" s="1">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="K19" s="1">
         <v>2</v>
@@ -2544,28 +2469,26 @@
       <c r="L19" s="1">
         <v>60</v>
       </c>
-      <c r="M19" s="1">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M19" s="20"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>113</v>
+        <v>31</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>111</v>
+        <v>7</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>100</v>
       </c>
       <c r="G20" s="1">
         <v>6</v>
@@ -2577,7 +2500,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="1">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="K20" s="1">
         <v>2</v>
@@ -2585,28 +2508,26 @@
       <c r="L20" s="1">
         <v>60</v>
       </c>
-      <c r="M20" s="1">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M20" s="20"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>107</v>
+        <v>15</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>103</v>
       </c>
       <c r="G21" s="1">
         <v>6</v>
@@ -2618,7 +2539,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="K21" s="1">
         <v>2</v>
@@ -2626,29 +2547,25 @@
       <c r="L21" s="1">
         <v>60</v>
       </c>
-      <c r="M21" s="1">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M21" s="20"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>92</v>
+      <c r="B22" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>110</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F22" s="15"/>
       <c r="G22" s="1">
         <v>6</v>
       </c>
@@ -2656,10 +2573,10 @@
         <v>3</v>
       </c>
       <c r="I22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" s="1">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="K22" s="1">
         <v>2</v>
@@ -2667,29 +2584,25 @@
       <c r="L22" s="1">
         <v>60</v>
       </c>
-      <c r="M22" s="1">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M22" s="20"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>103</v>
+        <v>218</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>119</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="15"/>
       <c r="G23" s="1">
         <v>6</v>
       </c>
@@ -2700,37 +2613,31 @@
         <v>0</v>
       </c>
       <c r="J23" s="1">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="K23" s="1">
-        <v>2</v>
-      </c>
-      <c r="L23" s="1">
-        <v>60</v>
-      </c>
-      <c r="M23" s="1">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1"/>
+      <c r="M23" s="20"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>95</v>
+        <v>219</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>119</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F24" s="11"/>
       <c r="G24" s="1">
         <v>6</v>
       </c>
@@ -2741,168 +2648,128 @@
         <v>0</v>
       </c>
       <c r="J24" s="1">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="K24" s="1">
         <v>0</v>
       </c>
       <c r="L24" s="1"/>
-      <c r="M24" s="1">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="G25" s="1">
-        <v>6</v>
-      </c>
-      <c r="H25" s="1">
-        <v>3</v>
-      </c>
-      <c r="I25" s="1">
-        <v>0</v>
-      </c>
-      <c r="J25" s="1">
-        <v>60</v>
-      </c>
-      <c r="K25" s="1">
-        <v>0</v>
-      </c>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1">
-        <v>440</v>
-      </c>
+      <c r="M24" s="20"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
-    <col min="4" max="4" width="41.109375" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" customWidth="1"/>
-    <col min="6" max="6" width="38.5546875" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="41.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="38.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" customWidth="1"/>
-    <col min="14" max="14" width="12.77734375" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" t="s">
         <v>114</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="E2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" t="s">
         <v>115</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D3" t="s">
-        <v>126</v>
-      </c>
       <c r="F3" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -2917,18 +2784,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="F4" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -2943,76 +2810,76 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D5" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="E5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F5" t="s">
+        <v>207</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" t="s">
+        <v>120</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" t="s">
         <v>130</v>
       </c>
-      <c r="F5" t="s">
-        <v>218</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E6" t="s">
-        <v>131</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D7" t="s">
-        <v>141</v>
-      </c>
       <c r="E7" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="F7" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="G7">
         <v>3</v>
@@ -3023,14 +2890,8 @@
       <c r="I7">
         <v>1</v>
       </c>
-      <c r="J7">
-        <v>120</v>
-      </c>
       <c r="K7">
         <v>2</v>
-      </c>
-      <c r="L7">
-        <v>60</v>
       </c>
       <c r="M7">
         <v>430</v>
@@ -3039,21 +2900,21 @@
         <v>353</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E8" t="s">
         <v>136</v>
       </c>
-      <c r="D8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E8" t="s">
-        <v>147</v>
-      </c>
       <c r="F8" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="G8">
         <v>3</v>
@@ -3064,14 +2925,8 @@
       <c r="I8">
         <v>1</v>
       </c>
-      <c r="J8">
-        <v>120</v>
-      </c>
       <c r="K8">
         <v>2</v>
-      </c>
-      <c r="L8">
-        <v>60</v>
       </c>
       <c r="M8">
         <v>430</v>
@@ -3080,19 +2935,19 @@
         <v>420</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" t="s">
+        <v>132</v>
+      </c>
+      <c r="E9" t="s">
         <v>137</v>
       </c>
-      <c r="D9" t="s">
-        <v>143</v>
-      </c>
-      <c r="E9" t="s">
-        <v>148</v>
-      </c>
       <c r="G9">
         <v>3</v>
       </c>
@@ -3101,9 +2956,6 @@
       </c>
       <c r="I9">
         <v>0</v>
-      </c>
-      <c r="J9">
-        <v>120</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -3112,21 +2964,21 @@
         <v>430</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="D10" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="G10">
         <v>3</v>
@@ -3137,14 +2989,8 @@
       <c r="I10">
         <v>1</v>
       </c>
-      <c r="J10">
-        <v>120</v>
-      </c>
       <c r="K10">
         <v>2</v>
-      </c>
-      <c r="L10">
-        <v>60</v>
       </c>
       <c r="M10">
         <v>430</v>
@@ -3153,18 +2999,18 @@
         <v>324</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="D11" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="E11" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="G11">
         <v>3</v>
@@ -3174,9 +3020,6 @@
       </c>
       <c r="I11">
         <v>0</v>
-      </c>
-      <c r="J11">
-        <v>120</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -3185,21 +3028,21 @@
         <v>430</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="D12" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="E12" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="F12" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="G12">
         <v>3</v>
@@ -3209,9 +3052,6 @@
       </c>
       <c r="I12">
         <v>0</v>
-      </c>
-      <c r="J12">
-        <v>120</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -3220,21 +3060,21 @@
         <v>430</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="D13" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="E13" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="F13" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="G13">
         <v>5</v>
@@ -3245,34 +3085,25 @@
       <c r="I13">
         <v>1</v>
       </c>
-      <c r="J13">
-        <v>120</v>
-      </c>
       <c r="K13">
         <v>2</v>
-      </c>
-      <c r="L13">
-        <v>60</v>
       </c>
       <c r="M13">
         <v>432</v>
       </c>
-      <c r="N13">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="D14" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="E14" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="G14">
         <v>5</v>
@@ -3283,9 +3114,6 @@
       <c r="I14">
         <v>0</v>
       </c>
-      <c r="J14">
-        <v>120</v>
-      </c>
       <c r="K14">
         <v>0</v>
       </c>
@@ -3293,21 +3121,21 @@
         <v>432</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D15" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="E15" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="F15" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="G15">
         <v>5</v>
@@ -3318,84 +3146,68 @@
       <c r="I15">
         <v>1</v>
       </c>
-      <c r="J15">
-        <v>120</v>
-      </c>
       <c r="K15">
         <v>2</v>
-      </c>
-      <c r="L15">
-        <v>60</v>
       </c>
       <c r="M15">
         <v>432</v>
       </c>
-      <c r="N15">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="G16" s="13">
+    </row>
+    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="G16" s="12">
         <v>5</v>
       </c>
-      <c r="H16" s="13">
-        <v>3</v>
-      </c>
-      <c r="I16" s="13">
-        <v>1</v>
-      </c>
-      <c r="J16" s="13">
-        <v>120</v>
-      </c>
-      <c r="K16" s="13">
-        <v>2</v>
-      </c>
-      <c r="L16">
-        <v>60</v>
-      </c>
+      <c r="H16" s="12">
+        <v>3</v>
+      </c>
+      <c r="I16" s="12">
+        <v>1</v>
+      </c>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12">
+        <v>2</v>
+      </c>
+      <c r="L16" s="12"/>
       <c r="M16">
         <v>432</v>
       </c>
-      <c r="N16" s="13">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C17" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D17" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="E17" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="F17" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G17">
         <v>5</v>
@@ -3406,40 +3218,31 @@
       <c r="I17">
         <v>1</v>
       </c>
-      <c r="J17">
-        <v>120</v>
-      </c>
       <c r="K17">
         <v>2</v>
-      </c>
-      <c r="L17">
-        <v>60</v>
       </c>
       <c r="M17">
         <v>432</v>
       </c>
-      <c r="N17">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="C18" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D18" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="E18" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="F18" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G18">
         <v>5</v>
@@ -3450,37 +3253,28 @@
       <c r="I18">
         <v>1</v>
       </c>
-      <c r="J18">
-        <v>120</v>
-      </c>
       <c r="K18">
         <v>2</v>
-      </c>
-      <c r="L18">
-        <v>60</v>
       </c>
       <c r="M18">
         <v>432</v>
       </c>
-      <c r="N18">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C19" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D19" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G19">
         <v>5</v>
@@ -3491,40 +3285,31 @@
       <c r="I19">
         <v>1</v>
       </c>
-      <c r="J19">
-        <v>60</v>
-      </c>
       <c r="K19">
         <v>2</v>
       </c>
-      <c r="L19">
-        <v>60</v>
-      </c>
       <c r="M19">
-        <v>326</v>
-      </c>
-      <c r="N19">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="C20" t="s">
+        <v>181</v>
+      </c>
+      <c r="D20" t="s">
+        <v>173</v>
+      </c>
+      <c r="E20" t="s">
+        <v>187</v>
+      </c>
+      <c r="F20" t="s">
         <v>192</v>
-      </c>
-      <c r="D20" t="s">
-        <v>184</v>
-      </c>
-      <c r="E20" t="s">
-        <v>198</v>
-      </c>
-      <c r="F20" t="s">
-        <v>203</v>
       </c>
       <c r="G20">
         <v>7</v>
@@ -3535,40 +3320,31 @@
       <c r="I20">
         <v>1</v>
       </c>
-      <c r="J20">
-        <v>120</v>
-      </c>
       <c r="K20">
         <v>2</v>
-      </c>
-      <c r="L20">
-        <v>60</v>
       </c>
       <c r="M20">
         <v>440</v>
       </c>
-      <c r="N20">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C21" t="s">
+        <v>182</v>
+      </c>
+      <c r="D21" t="s">
+        <v>174</v>
+      </c>
+      <c r="E21" t="s">
+        <v>160</v>
+      </c>
+      <c r="F21" t="s">
         <v>193</v>
-      </c>
-      <c r="D21" t="s">
-        <v>185</v>
-      </c>
-      <c r="E21" t="s">
-        <v>171</v>
-      </c>
-      <c r="F21" t="s">
-        <v>204</v>
       </c>
       <c r="G21">
         <v>7</v>
@@ -3579,40 +3355,31 @@
       <c r="I21">
         <v>1</v>
       </c>
-      <c r="J21">
-        <v>120</v>
-      </c>
       <c r="K21">
         <v>2</v>
-      </c>
-      <c r="L21">
-        <v>60</v>
       </c>
       <c r="M21">
         <v>440</v>
       </c>
-      <c r="N21">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="C22" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="D22" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="E22" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="F22" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="G22">
         <v>7</v>
@@ -3623,40 +3390,31 @@
       <c r="I22">
         <v>1</v>
       </c>
-      <c r="J22">
-        <v>120</v>
-      </c>
       <c r="K22">
         <v>2</v>
-      </c>
-      <c r="L22">
-        <v>60</v>
       </c>
       <c r="M22">
         <v>440</v>
       </c>
-      <c r="N22">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="C23" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="D23" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="E23" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="F23" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G23">
         <v>7</v>
@@ -3667,37 +3425,31 @@
       <c r="I23">
         <v>1</v>
       </c>
-      <c r="J23">
-        <v>60</v>
-      </c>
       <c r="K23">
         <v>2</v>
       </c>
-      <c r="L23">
-        <v>60</v>
-      </c>
       <c r="M23">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="C24" t="s">
+        <v>182</v>
+      </c>
+      <c r="D24" t="s">
+        <v>174</v>
+      </c>
+      <c r="E24" t="s">
+        <v>160</v>
+      </c>
+      <c r="F24" t="s">
         <v>193</v>
-      </c>
-      <c r="D24" t="s">
-        <v>185</v>
-      </c>
-      <c r="E24" t="s">
-        <v>171</v>
-      </c>
-      <c r="F24" t="s">
-        <v>204</v>
       </c>
       <c r="G24">
         <v>7</v>
@@ -3708,40 +3460,31 @@
       <c r="I24">
         <v>1</v>
       </c>
-      <c r="J24">
-        <v>120</v>
-      </c>
       <c r="K24">
         <v>2</v>
-      </c>
-      <c r="L24">
-        <v>60</v>
       </c>
       <c r="M24">
         <v>440</v>
       </c>
-      <c r="N24">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B25" t="s">
+        <v>166</v>
+      </c>
+      <c r="C25" t="s">
+        <v>183</v>
+      </c>
+      <c r="D25" t="s">
         <v>177</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E25" t="s">
+        <v>150</v>
+      </c>
+      <c r="F25" t="s">
         <v>194</v>
-      </c>
-      <c r="D25" t="s">
-        <v>188</v>
-      </c>
-      <c r="E25" t="s">
-        <v>161</v>
-      </c>
-      <c r="F25" t="s">
-        <v>205</v>
       </c>
       <c r="G25">
         <v>7</v>
@@ -3752,37 +3495,31 @@
       <c r="I25">
         <v>1</v>
       </c>
-      <c r="J25">
-        <v>60</v>
-      </c>
       <c r="K25">
         <v>2</v>
       </c>
-      <c r="L25">
-        <v>60</v>
-      </c>
       <c r="M25">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B26" t="s">
+        <v>167</v>
+      </c>
+      <c r="C26" t="s">
+        <v>181</v>
+      </c>
+      <c r="D26" t="s">
         <v>178</v>
       </c>
-      <c r="C26" t="s">
-        <v>192</v>
-      </c>
-      <c r="D26" t="s">
-        <v>189</v>
-      </c>
       <c r="E26" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="F26" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G26">
         <v>7</v>
@@ -3793,40 +3530,31 @@
       <c r="I26">
         <v>1</v>
       </c>
-      <c r="J26">
-        <v>60</v>
-      </c>
       <c r="K26">
         <v>2</v>
       </c>
-      <c r="L26">
-        <v>60</v>
-      </c>
       <c r="M26">
-        <v>438</v>
-      </c>
-      <c r="N26">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B27" t="s">
+        <v>168</v>
+      </c>
+      <c r="C27" t="s">
+        <v>182</v>
+      </c>
+      <c r="D27" t="s">
         <v>179</v>
       </c>
-      <c r="C27" t="s">
-        <v>193</v>
-      </c>
-      <c r="D27" t="s">
-        <v>190</v>
-      </c>
       <c r="E27" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="F27" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="G27">
         <v>7</v>
@@ -3837,40 +3565,31 @@
       <c r="I27">
         <v>1</v>
       </c>
-      <c r="J27">
-        <v>60</v>
-      </c>
       <c r="K27">
         <v>2</v>
       </c>
-      <c r="L27">
-        <v>60</v>
-      </c>
       <c r="M27">
-        <v>438</v>
-      </c>
-      <c r="N27">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="C28" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="D28" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F28" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="G28">
         <v>7</v>
@@ -3881,40 +3600,31 @@
       <c r="I28">
         <v>1</v>
       </c>
-      <c r="J28">
-        <v>60</v>
-      </c>
       <c r="K28">
         <v>2</v>
       </c>
-      <c r="L28">
-        <v>60</v>
-      </c>
       <c r="M28">
-        <v>438</v>
-      </c>
-      <c r="N28">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B29" t="s">
+        <v>170</v>
+      </c>
+      <c r="C29" t="s">
         <v>181</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
+        <v>185</v>
+      </c>
+      <c r="E29" t="s">
+        <v>189</v>
+      </c>
+      <c r="F29" t="s">
         <v>192</v>
-      </c>
-      <c r="D29" t="s">
-        <v>196</v>
-      </c>
-      <c r="E29" t="s">
-        <v>200</v>
-      </c>
-      <c r="F29" t="s">
-        <v>203</v>
       </c>
       <c r="G29">
         <v>7</v>
@@ -3925,37 +3635,28 @@
       <c r="I29">
         <v>1</v>
       </c>
-      <c r="J29">
-        <v>60</v>
-      </c>
       <c r="K29">
         <v>2</v>
       </c>
-      <c r="L29">
-        <v>60</v>
-      </c>
       <c r="M29">
-        <v>431</v>
-      </c>
-      <c r="N29">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B30" t="s">
+        <v>171</v>
+      </c>
+      <c r="C30" t="s">
         <v>182</v>
       </c>
-      <c r="C30" t="s">
-        <v>193</v>
-      </c>
       <c r="D30" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="E30" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="G30">
         <v>7</v>
@@ -3966,40 +3667,31 @@
       <c r="I30">
         <v>1</v>
       </c>
-      <c r="J30">
-        <v>60</v>
-      </c>
       <c r="K30">
         <v>2</v>
       </c>
-      <c r="L30">
-        <v>60</v>
-      </c>
       <c r="M30">
-        <v>431</v>
-      </c>
-      <c r="N30">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B31" t="s">
+        <v>172</v>
+      </c>
+      <c r="C31" t="s">
         <v>183</v>
       </c>
-      <c r="C31" t="s">
-        <v>194</v>
-      </c>
       <c r="D31" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="E31" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="F31" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="G31">
         <v>7</v>
@@ -4010,35 +3702,26 @@
       <c r="I31">
         <v>1</v>
       </c>
-      <c r="J31">
-        <v>60</v>
-      </c>
       <c r="K31">
         <v>2</v>
       </c>
-      <c r="L31">
-        <v>60</v>
-      </c>
       <c r="M31">
-        <v>431</v>
-      </c>
-      <c r="N31">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
     </row>
   </sheetData>
@@ -4048,810 +3731,282 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C4" s="4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C5" s="4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="4">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C6" s="4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="4">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C7" s="4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="4">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="B8" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="4">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="C8" s="4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C9" s="4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="4">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="B10" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C10" s="4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="4">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C11" s="4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="4">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C12" s="4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="4">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="C13" s="4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="4">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="B14" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C14" s="4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="4">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="B15" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="C15" s="4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="4">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="B16" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="C16" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="4">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="4">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="4">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="C17" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C18" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C19" s="4">
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C20" s="4">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C21" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C22" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C23" s="4">
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C24" s="4">
         <v>120</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N20"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="42.33203125" customWidth="1"/>
-    <col min="5" max="5" width="19.88671875" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" customWidth="1"/>
-    <col min="14" max="14" width="14.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>227</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>229</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>242</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>120</v>
-      </c>
-      <c r="K2">
-        <v>3</v>
-      </c>
-      <c r="L2">
-        <v>60</v>
-      </c>
-      <c r="M2">
-        <v>409</v>
-      </c>
-      <c r="N2">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>227</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>230</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>231</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>232</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>242</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>3</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>120</v>
-      </c>
-      <c r="K3">
-        <v>3</v>
-      </c>
-      <c r="L3">
-        <v>60</v>
-      </c>
-      <c r="M3">
-        <v>409</v>
-      </c>
-      <c r="N3">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>227</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>233</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>235</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>243</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>120</v>
-      </c>
-      <c r="K4">
-        <v>3</v>
-      </c>
-      <c r="L4">
-        <v>60</v>
-      </c>
-      <c r="M4">
-        <v>409</v>
-      </c>
-      <c r="N4">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>227</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>120</v>
-      </c>
-      <c r="K5">
-        <v>2</v>
-      </c>
-      <c r="L5">
-        <v>60</v>
-      </c>
-      <c r="M5">
-        <v>409</v>
-      </c>
-      <c r="N5">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>227</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>240</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>241</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6">
-        <v>3</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>120</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>60</v>
-      </c>
-      <c r="M6">
-        <v>409</v>
-      </c>
-      <c r="N6">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>227</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="G7">
-        <v>4</v>
-      </c>
-      <c r="H7">
-        <v>3</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>120</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>60</v>
-      </c>
-      <c r="M7">
-        <v>409</v>
-      </c>
-      <c r="N7">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>227</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>248</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>232</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>242</v>
-      </c>
-      <c r="G8">
-        <v>4</v>
-      </c>
-      <c r="H8">
-        <v>3</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>120</v>
-      </c>
-      <c r="K8">
-        <v>2</v>
-      </c>
-      <c r="L8">
-        <v>60</v>
-      </c>
-      <c r="M8">
-        <v>409</v>
-      </c>
-      <c r="N8">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>227</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>250</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>251</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>242</v>
-      </c>
-      <c r="G9">
-        <v>4</v>
-      </c>
-      <c r="H9">
-        <v>3</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>120</v>
-      </c>
-      <c r="K9">
-        <v>2</v>
-      </c>
-      <c r="L9">
-        <v>60</v>
-      </c>
-      <c r="M9">
-        <v>409</v>
-      </c>
-      <c r="N9">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>227</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>253</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>254</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>258</v>
-      </c>
-      <c r="G10">
-        <v>4</v>
-      </c>
-      <c r="H10">
-        <v>3</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>120</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>60</v>
-      </c>
-      <c r="M10">
-        <v>409</v>
-      </c>
-      <c r="N10">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>227</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>256</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>257</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>258</v>
-      </c>
-      <c r="G11">
-        <v>4</v>
-      </c>
-      <c r="H11">
-        <v>3</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>120</v>
-      </c>
-      <c r="K11">
-        <v>2</v>
-      </c>
-      <c r="L11">
-        <v>60</v>
-      </c>
-      <c r="M11">
-        <v>409</v>
-      </c>
-      <c r="N11">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>227</v>
-      </c>
-      <c r="J12">
-        <v>120</v>
-      </c>
-      <c r="L12">
-        <v>60</v>
-      </c>
-      <c r="M12">
-        <v>409</v>
-      </c>
-      <c r="N12">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>